<commit_message>
update toxic no obs
</commit_message>
<xml_diff>
--- a/help/27_COVID_19_regiz.xlsx
+++ b/help/27_COVID_19_regiz.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharinM\Desktop\Загрузки_временные\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Загрузки_временные\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="133">
   <si>
     <t>Лаборатория</t>
   </si>
@@ -465,6 +465,9 @@
   <si>
     <t>ФГКУ «Поликлиника №4 Федеральной таможенной службы»</t>
   </si>
+  <si>
+    <t>ООО "Сиквенс"</t>
+  </si>
 </sst>
 </file>
 
@@ -773,7 +776,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -1383,6 +1386,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
@@ -1398,7 +1414,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1735,6 +1751,21 @@
     </xf>
     <xf numFmtId="3" fontId="20" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="5" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="17" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="11" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2439,10 +2470,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G16" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2457,19 +2488,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="133" t="s">
+      <c r="E1" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="134"/>
-      <c r="G1" s="133" t="s">
+      <c r="F1" s="139"/>
+      <c r="G1" s="138" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="134"/>
-      <c r="I1" s="121" t="s">
+      <c r="H1" s="139"/>
+      <c r="I1" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="122"/>
-      <c r="K1" s="123"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="128"/>
     </row>
     <row r="2" spans="1:11" ht="153" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67" t="s">
@@ -2538,12 +2569,12 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="126"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="131"/>
       <c r="E4" s="78" t="e">
         <f>E5+E52</f>
         <v>#N/A</v>
@@ -2565,12 +2596,12 @@
       <c r="K4" s="81"/>
     </row>
     <row r="5" spans="1:11" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="127" t="s">
+      <c r="A5" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="129"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="134"/>
       <c r="E5" s="72" t="e">
         <f>E6+E9+E37</f>
         <v>#N/A</v>
@@ -2592,12 +2623,12 @@
       <c r="K5" s="73"/>
     </row>
     <row r="6" spans="1:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="130" t="s">
+      <c r="A6" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="131"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="132"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="137"/>
       <c r="E6" s="74" t="e">
         <f>SUM(E7:E8)</f>
         <v>#N/A</v>
@@ -2694,11 +2725,11 @@
         <v/>
       </c>
       <c r="I8" s="51" t="e">
-        <f t="shared" ref="I8:I72" si="1">IFERROR($E8-$G8,IF(ISBLANK($E8),$G8,$E8))</f>
+        <f t="shared" ref="I8:I73" si="1">IFERROR($E8-$G8,IF(ISBLANK($E8),$G8,$E8))</f>
         <v>#N/A</v>
       </c>
       <c r="J8" s="52" t="e">
-        <f t="shared" ref="J8:J72" si="2">IFERROR($F8-$H8,IF(ISBLANK($F8),$H8,$F8))</f>
+        <f t="shared" ref="J8:J73" si="2">IFERROR($F8-$H8,IF(ISBLANK($F8),$H8,$F8))</f>
         <v>#N/A</v>
       </c>
       <c r="K8" s="52" t="e">
@@ -4476,7 +4507,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="162.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="186" x14ac:dyDescent="0.25">
       <c r="A50" s="56">
         <v>42</v>
       </c>
@@ -4572,19 +4603,19 @@
         <v>109</v>
       </c>
       <c r="E52" s="63" t="e">
-        <f>SUM(E53:E72)</f>
+        <f>SUM(E53:E73)</f>
         <v>#N/A</v>
       </c>
       <c r="F52" s="63" t="e">
-        <f>SUM(F53:F72)</f>
+        <f>SUM(F53:F73)</f>
         <v>#N/A</v>
       </c>
       <c r="G52" s="63">
-        <f>SUM(G53:G72)</f>
+        <f>SUM(G53:G73)</f>
         <v>0</v>
       </c>
       <c r="H52" s="63">
-        <f>SUM(H53:H72)</f>
+        <f>SUM(H53:H73)</f>
         <v>0</v>
       </c>
       <c r="I52" s="62"/>
@@ -5426,47 +5457,91 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="64">
+    <row r="72" spans="1:11" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="121">
         <v>63</v>
       </c>
-      <c r="B72" s="103" t="e">
+      <c r="B72" s="122" t="e">
         <f>VLOOKUP($D72,parus!$A:$AA,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="C72" s="103" t="s">
+      <c r="C72" s="122" t="s">
         <v>128</v>
       </c>
-      <c r="D72" s="103" t="s">
+      <c r="D72" s="122" t="s">
         <v>127</v>
       </c>
-      <c r="E72" s="117" t="e">
+      <c r="E72" s="123" t="e">
         <f>VLOOKUP($D72,parus!$A$3:$AA$100,21,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F72" s="118" t="e">
+      <c r="F72" s="124" t="e">
         <f>VLOOKUP($D72,parus!$A$3:$AA$100,23,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="G72" s="117" t="str">
+      <c r="G72" s="123" t="str">
         <f>IFERROR(VLOOKUP($C72,regiz!$B:$J,4,0),"")</f>
         <v/>
       </c>
-      <c r="H72" s="118" t="str">
+      <c r="H72" s="124" t="str">
         <f>IFERROR(VLOOKUP($C72,regiz!$B:$J,5,0),"")</f>
         <v/>
       </c>
-      <c r="I72" s="119" t="e">
+      <c r="I72" s="125" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="J72" s="119" t="e">
+      <c r="J72" s="125" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="K72" s="52" t="str">
+      <c r="K72" s="98" t="str">
         <f>IF(C72=0, "нет в РЕГИЗе","есть")</f>
         <v>есть</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="64">
+        <v>63</v>
+      </c>
+      <c r="B73" s="103" t="e">
+        <f>VLOOKUP($D73,parus!$A:$AA,2,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C73" s="103" t="e">
+        <f>IF(B73=0,0,VLOOKUP($B73,nsi!$F:$G,2,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D73" s="103" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" s="117" t="e">
+        <f>VLOOKUP($D73,parus!$A$3:$AA$100,21,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F73" s="118" t="e">
+        <f>VLOOKUP($D73,parus!$A$3:$AA$100,23,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G73" s="117" t="str">
+        <f>IFERROR(VLOOKUP($C73,regiz!$B:$J,4,0),"")</f>
+        <v/>
+      </c>
+      <c r="H73" s="118" t="str">
+        <f>IFERROR(VLOOKUP($C73,regiz!$B:$J,5,0),"")</f>
+        <v/>
+      </c>
+      <c r="I73" s="119" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="J73" s="119" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="K73" s="52" t="e">
+        <f>IF(C73=0, "нет в РЕГИЗе","есть")</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -5511,107 +5586,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="153" t="s">
+      <c r="B1" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="155" t="s">
+      <c r="C1" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="156" t="s">
+      <c r="D1" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="157" t="s">
+      <c r="E1" s="162" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="143" t="s">
+      <c r="F1" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="145" t="s">
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="149"/>
+      <c r="M1" s="149"/>
+      <c r="N1" s="149"/>
+      <c r="O1" s="143"/>
+      <c r="P1" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="145" t="s">
+      <c r="Q1" s="150" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="145" t="s">
+      <c r="R1" s="150" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="138"/>
-      <c r="T1" s="147" t="s">
+      <c r="S1" s="143"/>
+      <c r="T1" s="152" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="138"/>
-      <c r="V1" s="148" t="s">
+      <c r="U1" s="143"/>
+      <c r="V1" s="153" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="138"/>
-      <c r="X1" s="149" t="s">
+      <c r="W1" s="143"/>
+      <c r="X1" s="154" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="138"/>
-      <c r="Z1" s="146" t="s">
+      <c r="Y1" s="143"/>
+      <c r="Z1" s="151" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="146" t="s">
+      <c r="AA1" s="151" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="152" t="s">
+      <c r="AB1" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="140" t="s">
+      <c r="AC1" s="145" t="s">
         <v>29</v>
       </c>
       <c r="AD1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="150"/>
-      <c r="AF1" s="141" t="s">
+      <c r="AE1" s="155"/>
+      <c r="AF1" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="AG1" s="142" t="s">
+      <c r="AG1" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="AH1" s="135" t="s">
+      <c r="AH1" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="AI1" s="137" t="s">
+      <c r="AI1" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="AJ1" s="137" t="s">
+      <c r="AJ1" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="AK1" s="137" t="s">
+      <c r="AK1" s="142" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" s="138"/>
+      <c r="AL1" s="143"/>
       <c r="AM1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AN1" s="139" t="s">
+      <c r="AN1" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="AO1" s="138"/>
+      <c r="AO1" s="143"/>
       <c r="AP1" s="26" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:42" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136"/>
-      <c r="B2" s="136"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
+      <c r="A2" s="141"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
       <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
@@ -5642,8 +5717,8 @@
       <c r="O2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="136"/>
-      <c r="Q2" s="136"/>
+      <c r="P2" s="141"/>
+      <c r="Q2" s="141"/>
       <c r="R2" s="11" t="s">
         <v>17</v>
       </c>
@@ -5668,19 +5743,19 @@
       <c r="Y2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="136"/>
-      <c r="AA2" s="136"/>
-      <c r="AB2" s="136"/>
-      <c r="AC2" s="136"/>
+      <c r="Z2" s="141"/>
+      <c r="AA2" s="141"/>
+      <c r="AB2" s="141"/>
+      <c r="AC2" s="141"/>
       <c r="AD2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AE2" s="151"/>
-      <c r="AF2" s="136"/>
-      <c r="AG2" s="136"/>
-      <c r="AH2" s="136"/>
-      <c r="AI2" s="136"/>
-      <c r="AJ2" s="136"/>
+      <c r="AE2" s="156"/>
+      <c r="AF2" s="141"/>
+      <c r="AG2" s="141"/>
+      <c r="AH2" s="141"/>
+      <c r="AI2" s="141"/>
+      <c r="AJ2" s="141"/>
       <c r="AK2" s="18" t="s">
         <v>17</v>
       </c>
@@ -5813,7 +5888,7 @@
         <f t="shared" ref="AD3" si="2">W3-Y3</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="136"/>
+      <c r="AE3" s="141"/>
       <c r="AF3" s="27">
         <f t="shared" ref="AF3" si="3">IF(C3&gt;=U3,0,1)</f>
         <v>0</v>

</xml_diff>